<commit_message>
Add USB host driver
</commit_message>
<xml_diff>
--- a/DesignDocument/LCD/LCD Screen Design.xlsx
+++ b/DesignDocument/LCD/LCD Screen Design.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33AB569-ABF1-451D-9059-887B5365342F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458ADEC6-26DC-4802-8CE4-DBB6B2BA1907}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Old" sheetId="2" r:id="rId1"/>
     <sheet name="New" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,9 +22,166 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="38">
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I/t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,16 +196,50 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -54,12 +247,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -145,6 +636,907 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.3233814523184596E-2"/>
+          <c:y val="0.1551362683438155"/>
+          <c:w val="0.88621062992125987"/>
+          <c:h val="0.65168391686888205"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AV$13:$AV$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-04CB-45B5-A3C4-03A2448824A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AW$13:$AW$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-04CB-45B5-A3C4-03A2448824A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="768160000"/>
+        <c:axId val="768160328"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="768160000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="768160328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="768160328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="768160000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.35868897637795277"/>
+          <c:y val="5.7815689705449278E-4"/>
+          <c:w val="0.31039982502187224"/>
+          <c:h val="7.7540908931383865E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -183,6 +1575,94 @@
         <a:xfrm>
           <a:off x="2333297" y="0"/>
           <a:ext cx="4314496" cy="2645251"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>593170</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>131380</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123977</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>141015</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82D7C792-D338-409C-A4A1-EF5C40B281D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2421970" y="2732690"/>
+          <a:ext cx="3188407" cy="2090684"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2902</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>52297</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>405127</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133608</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E264CAA-FF35-4496-BC61-6AA97E2CABA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5489302" y="3019181"/>
+          <a:ext cx="2840625" cy="2001059"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1624,6 +3104,370 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="直接连接符 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DC31C6C-6065-42BA-84AF-2A0FAE76EB3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="342900" y="388620"/>
+          <a:ext cx="3566160" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直接箭头连接符 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D1B646C-B02F-4EEA-87CB-72FF6A7147FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3627120" y="533400"/>
+          <a:ext cx="0" cy="4114800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直接箭头连接符 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCB7F509-E8C4-468E-9B8E-ADDA483DDB64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6484620" y="533400"/>
+          <a:ext cx="0" cy="4114800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="直接连接符 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F197966-B049-445C-BAE9-AEC1BFC6177E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4198620" y="617220"/>
+          <a:ext cx="525780" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="直接连接符 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F46E33C4-6330-47B3-9BD4-D4CA807BC45A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5349240" y="617220"/>
+          <a:ext cx="525780" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="20" name="图表 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{782D45B7-560B-4302-91B2-4E8F9F0C79AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161108</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>13062</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="直接箭头连接符 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7DF0423-0CB8-4692-81F3-44DE6C889371}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2194560" y="2760617"/>
+          <a:ext cx="1637211" cy="8709"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1632,7 +3476,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACE"/>
+        <a:sysClr val="window" lastClr="CEEACA"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1889,8 +3733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBCE5484-8812-4A90-B5C2-E047ED27A05F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1905,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236968F1-8EC4-4E81-BA2A-42A7E714686E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1915,4 +3759,1295 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C00CABF-CD5F-438D-823F-38C2E845CE61}">
+  <dimension ref="A1:AW33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="AA34" sqref="AA34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="42" width="1.33203125" customWidth="1"/>
+    <col min="43" max="44" width="2.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:49" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2">
+        <v>40</v>
+      </c>
+      <c r="H1" s="2">
+        <v>48</v>
+      </c>
+      <c r="I1" s="2">
+        <v>56</v>
+      </c>
+      <c r="J1" s="2">
+        <v>64</v>
+      </c>
+      <c r="K1" s="2">
+        <v>72</v>
+      </c>
+      <c r="L1" s="2">
+        <v>80</v>
+      </c>
+      <c r="M1" s="2">
+        <v>88</v>
+      </c>
+      <c r="N1" s="2">
+        <v>96</v>
+      </c>
+      <c r="O1" s="2">
+        <v>104</v>
+      </c>
+      <c r="P1" s="2">
+        <v>112</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>120</v>
+      </c>
+      <c r="R1" s="2">
+        <v>128</v>
+      </c>
+      <c r="S1" s="2">
+        <v>136</v>
+      </c>
+      <c r="T1" s="2">
+        <v>144</v>
+      </c>
+      <c r="U1" s="2">
+        <v>152</v>
+      </c>
+      <c r="V1" s="2">
+        <v>160</v>
+      </c>
+      <c r="W1" s="2">
+        <v>168</v>
+      </c>
+      <c r="X1" s="2">
+        <v>176</v>
+      </c>
+      <c r="Y1" s="2">
+        <v>184</v>
+      </c>
+      <c r="Z1" s="2">
+        <v>192</v>
+      </c>
+      <c r="AA1" s="2">
+        <v>200</v>
+      </c>
+      <c r="AB1" s="2">
+        <v>208</v>
+      </c>
+      <c r="AC1" s="2">
+        <v>216</v>
+      </c>
+      <c r="AD1" s="2">
+        <v>224</v>
+      </c>
+      <c r="AE1" s="2">
+        <v>232</v>
+      </c>
+      <c r="AF1" s="2">
+        <v>240</v>
+      </c>
+      <c r="AG1" s="2">
+        <v>248</v>
+      </c>
+      <c r="AH1" s="2">
+        <v>256</v>
+      </c>
+      <c r="AI1" s="2">
+        <v>264</v>
+      </c>
+      <c r="AJ1" s="2">
+        <v>272</v>
+      </c>
+      <c r="AK1" s="2">
+        <v>280</v>
+      </c>
+      <c r="AL1" s="2">
+        <v>288</v>
+      </c>
+      <c r="AM1" s="2">
+        <v>296</v>
+      </c>
+      <c r="AN1" s="2">
+        <v>304</v>
+      </c>
+      <c r="AO1" s="2">
+        <v>312</v>
+      </c>
+      <c r="AP1" s="2">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="6"/>
+    </row>
+    <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="8"/>
+      <c r="AM3" s="8"/>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8"/>
+      <c r="AP3" s="10"/>
+    </row>
+    <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>32</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP4" s="10"/>
+    </row>
+    <row r="5" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>48</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
+      <c r="AK5" s="8"/>
+      <c r="AL5" s="8"/>
+      <c r="AM5" s="8"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8"/>
+      <c r="AP5" s="10"/>
+    </row>
+    <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>64</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="9">
+        <v>1</v>
+      </c>
+      <c r="L6" s="8">
+        <v>2</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+      <c r="AL6" s="8"/>
+      <c r="AM6" s="8"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="8"/>
+      <c r="AP6" s="10"/>
+    </row>
+    <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>80</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="8"/>
+      <c r="AJ7" s="8"/>
+      <c r="AK7" s="8"/>
+      <c r="AL7" s="8"/>
+      <c r="AM7" s="8"/>
+      <c r="AN7" s="8"/>
+      <c r="AO7" s="8"/>
+      <c r="AP7" s="10"/>
+    </row>
+    <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>96</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
+      <c r="AK8" s="8"/>
+      <c r="AL8" s="8"/>
+      <c r="AM8" s="8"/>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="10"/>
+    </row>
+    <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>112</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="8"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
+      <c r="AM9" s="8"/>
+      <c r="AN9" s="8"/>
+      <c r="AO9" s="8"/>
+      <c r="AP9" s="10"/>
+    </row>
+    <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>128</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
+      <c r="AJ10" s="8"/>
+      <c r="AK10" s="8"/>
+      <c r="AL10" s="8"/>
+      <c r="AM10" s="8"/>
+      <c r="AN10" s="8"/>
+      <c r="AO10" s="8"/>
+      <c r="AP10" s="10"/>
+    </row>
+    <row r="11" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>144</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
+      <c r="AI11" s="8"/>
+      <c r="AJ11" s="8"/>
+      <c r="AK11" s="8"/>
+      <c r="AL11" s="8"/>
+      <c r="AM11" s="8"/>
+      <c r="AN11" s="8"/>
+      <c r="AO11" s="8"/>
+      <c r="AP11" s="10"/>
+    </row>
+    <row r="12" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>160</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8">
+        <v>5</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="8">
+        <v>5</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>0</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="S12" s="8">
+        <v>2</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="8"/>
+      <c r="AE12" s="8"/>
+      <c r="AF12" s="8"/>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="8"/>
+      <c r="AI12" s="8"/>
+      <c r="AJ12" s="8"/>
+      <c r="AK12" s="8"/>
+      <c r="AL12" s="8"/>
+      <c r="AM12" s="8"/>
+      <c r="AN12" s="8"/>
+      <c r="AO12" s="8"/>
+      <c r="AP12" s="10"/>
+    </row>
+    <row r="13" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>176</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+      <c r="AC13" s="8"/>
+      <c r="AD13" s="8"/>
+      <c r="AE13" s="8"/>
+      <c r="AF13" s="8"/>
+      <c r="AG13" s="8"/>
+      <c r="AH13" s="8"/>
+      <c r="AI13" s="8"/>
+      <c r="AJ13" s="8"/>
+      <c r="AK13" s="8"/>
+      <c r="AL13" s="8"/>
+      <c r="AM13" s="8"/>
+      <c r="AN13" s="8"/>
+      <c r="AO13" s="8"/>
+      <c r="AP13" s="10"/>
+      <c r="AV13">
+        <v>0</v>
+      </c>
+      <c r="AW13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>192</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8">
+        <v>5</v>
+      </c>
+      <c r="N14" s="8">
+        <v>0</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="P14" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="8"/>
+      <c r="AI14" s="8"/>
+      <c r="AJ14" s="8"/>
+      <c r="AK14" s="8"/>
+      <c r="AL14" s="8"/>
+      <c r="AM14" s="8"/>
+      <c r="AN14" s="8"/>
+      <c r="AO14" s="8"/>
+      <c r="AP14" s="10"/>
+      <c r="AV14">
+        <v>2</v>
+      </c>
+      <c r="AW14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>208</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="8"/>
+      <c r="AD15" s="8"/>
+      <c r="AE15" s="8"/>
+      <c r="AF15" s="8"/>
+      <c r="AG15" s="8"/>
+      <c r="AH15" s="8"/>
+      <c r="AI15" s="8"/>
+      <c r="AJ15" s="8"/>
+      <c r="AK15" s="8"/>
+      <c r="AL15" s="8"/>
+      <c r="AM15" s="8"/>
+      <c r="AN15" s="8"/>
+      <c r="AO15" s="8"/>
+      <c r="AP15" s="10"/>
+      <c r="AV15">
+        <v>4</v>
+      </c>
+      <c r="AW15">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>224</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8">
+        <v>2</v>
+      </c>
+      <c r="J16" s="8">
+        <v>3</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="8">
+        <v>5</v>
+      </c>
+      <c r="M16" s="9">
+        <v>0</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="9">
+        <v>1</v>
+      </c>
+      <c r="P16" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="8"/>
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="8"/>
+      <c r="AH16" s="8"/>
+      <c r="AI16" s="8"/>
+      <c r="AJ16" s="8"/>
+      <c r="AK16" s="8"/>
+      <c r="AL16" s="8"/>
+      <c r="AM16" s="8"/>
+      <c r="AN16" s="8"/>
+      <c r="AO16" s="8"/>
+      <c r="AP16" s="10"/>
+      <c r="AV16">
+        <v>6</v>
+      </c>
+      <c r="AW16">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:49" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>240</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="12"/>
+      <c r="AB17" s="12"/>
+      <c r="AC17" s="12"/>
+      <c r="AD17" s="12"/>
+      <c r="AE17" s="12"/>
+      <c r="AF17" s="12"/>
+      <c r="AG17" s="12"/>
+      <c r="AH17" s="12"/>
+      <c r="AI17" s="12"/>
+      <c r="AJ17" s="12"/>
+      <c r="AK17" s="12"/>
+      <c r="AL17" s="12"/>
+      <c r="AM17" s="12"/>
+      <c r="AN17" s="12"/>
+      <c r="AO17" s="12"/>
+      <c r="AP17" s="13"/>
+      <c r="AV17">
+        <v>8</v>
+      </c>
+      <c r="AW17">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:49" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="14"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="U20" s="22"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+    </row>
+    <row r="21" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="14">
+        <v>212</v>
+      </c>
+      <c r="R21" s="24"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="25"/>
+      <c r="W21" s="19"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
+    </row>
+    <row r="22" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="14"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="18"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="19"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+    </row>
+    <row r="23" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="14"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="19"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+    </row>
+    <row r="24" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+    </row>
+    <row r="25" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="14"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="28"/>
+      <c r="W25" s="19"/>
+      <c r="X25" s="15"/>
+      <c r="Y25" s="15"/>
+    </row>
+    <row r="26" spans="1:49" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="14"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="31"/>
+      <c r="W26" s="19"/>
+      <c r="X26" s="15"/>
+      <c r="Y26" s="15"/>
+    </row>
+    <row r="27" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="14"/>
+      <c r="R27" s="20"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="20"/>
+      <c r="U27" s="20"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="15"/>
+      <c r="Y27" s="15"/>
+    </row>
+    <row r="28" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:49" ht="7.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="7.8" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5A183E-F678-493C-BC19-30CB5656C6DF}">
+  <dimension ref="B9:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>212</v>
+      </c>
+      <c r="C9">
+        <v>32</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <f>(B9-C9-24)/D9</f>
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>160</v>
+      </c>
+      <c r="C10">
+        <v>304</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <f>(B10-C10)/D10</f>
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>